<commit_message>
update manifests, date: 2021-02-12, last lines (exp, sim, neg): (47, 121, 26)
</commit_message>
<xml_diff>
--- a/manifests/Simulation_Manifest.xlsx
+++ b/manifests/Simulation_Manifest.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="36" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I69"/>
@@ -5250,6 +5250,805 @@
         </is>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>s103</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>s103_e29_24019-32_1_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>937</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>570</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>s104</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>s104_e30_24019-32_1_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>640</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>1027</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>s105</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>s105_e31_24019-32_1_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>1333</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>s106</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>s106_e32_24019-32_1_4.jpeg</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>1806</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>165</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>s107</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>s107_e33_24019-32_1_5.jpeg</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>192</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>405</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>s108</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>s108_e34_24019-32_1_6.jpeg</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>1688</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>378</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>s109</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>s109_e35_24019-32_1_7.jpeg</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>239</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>1089</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>s110</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>s110_e36_24019-32_1_8.jpeg</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>1781</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>1169</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>s111</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>s111_e37_24019-32_2_7.jpeg</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>1016</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>616</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>s112</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>s112_e38_24019-32_2_6.jpeg</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>507</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>652</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>s113</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>s113_e39_24019-32_2_5.jpeg</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>1081</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>1391</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>s114</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>s114_e40_24019-32_2_4.jpeg</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>1304</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>311</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>s115</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>s115_e41_24019-32_2_3.jpeg</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>647</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>425</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>s116</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>s116_e42_24019-32_2_2.jpeg</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>1497</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>1455</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>s117</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>s117_e43_24019-32_2_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>1763</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>182</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>s118</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>s118_e44_24019-32_2_0.jpeg</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>379</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>266</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>s119</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>s119_e45_24019-32_3_1.jpeg</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>meltpatch</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>572</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>